<commit_message>
update in polarized jets
improve naming of uncertainties in datasets 20002 and 20003
correct '%-beam-polarization_c' to '%-norm_c' for datasets 20005 and 20007, according to section IV.C.4 of STAR 2012 paper
remove duplicated systematics in dataset 20006
update readme.md file with above corrections
other minor updates
</commit_message>
<xml_diff>
--- a/pjets/expdata/20002.xlsx
+++ b/pjets/expdata/20002.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17020" tabRatio="500"/>
+    <workbookView windowHeight="17880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,13 +58,13 @@
     <t>stat_u</t>
   </si>
   <si>
-    <t>tri-jet_c</t>
+    <t>trigger-bias-jet_c</t>
   </si>
   <si>
     <t>nonlong_c</t>
   </si>
   <si>
-    <t>beam_c</t>
+    <t>beam-gas_c</t>
   </si>
   <si>
     <t>shift_c</t>
@@ -87,9 +87,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -118,9 +118,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,6 +139,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -141,9 +170,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -155,6 +192,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -165,14 +224,37 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -185,88 +267,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -277,19 +277,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -301,163 +397,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,21 +505,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -551,6 +536,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -559,160 +568,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1054,7 +1054,7 @@
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71120689655172" defaultRowHeight="24.4"/>
@@ -1065,7 +1065,9 @@
     <col min="9" max="9" width="14.8534482758621" customWidth="1"/>
     <col min="10" max="11" width="15.5689655172414" customWidth="1"/>
     <col min="12" max="12" width="7.85344827586207" customWidth="1"/>
-    <col min="13" max="17" width="17" customWidth="1"/>
+    <col min="13" max="14" width="17" customWidth="1"/>
+    <col min="15" max="15" width="20.8275862068966" customWidth="1"/>
+    <col min="16" max="17" width="17" customWidth="1"/>
     <col min="18" max="18" width="12.2844827586207" customWidth="1"/>
     <col min="19" max="19" width="12.8534482758621" customWidth="1"/>
     <col min="20" max="1023" width="10.2844827586207" customWidth="1"/>
@@ -1731,7 +1733,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>

</xml_diff>